<commit_message>
Reversed the colors of the stackplot. Corrected a mistace in household composition. HH type 2 consists of 2x person type 1.
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_HouseholdComposition.xlsx
+++ b/data/input_behavior/BehaviorScenario_HouseholdComposition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/PycharmProjects/FLEX/data/input_behavior/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C022983-0690-5949-9642-447EAEF8FE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9B4728-DE50-A14F-941D-D939F1CE25C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="-18880" windowWidth="22360" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -500,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -645,6 +645,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0f10bb0856646bfda2b94dc29ed0a887">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca21336e7eb6462c50ac4645cdd355ca" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -849,15 +858,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -870,6 +870,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C498-74B4-4650-B402-97A5D02496A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8831E31-2A91-4E0B-B823-0BFA5718552C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -888,14 +896,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C498-74B4-4650-B402-97A5D02496A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE03864-EF8F-45D0-B8AF-9F190340F3F6}">
   <ds:schemaRefs>

</xml_diff>